<commit_message>
corrected amplitude simulations in T & M
</commit_message>
<xml_diff>
--- a/DATA/model_compare.xlsx
+++ b/DATA/model_compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauraelsler/Dropbox/PhD/Resources/Squid/Squid/CODE/Squid/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536EB376-5F12-E041-BEC2-946127ED47E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE0E2E5-8690-B24A-84DA-87780893BDA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15520" xr2:uid="{1D73CAE5-B16D-354F-B7D4-C99306CF6EB3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="179">
   <si>
     <t>Year</t>
   </si>
@@ -556,6 +556,12 @@
   </si>
   <si>
     <t>1.129582887636718e-10</t>
+  </si>
+  <si>
+    <t>266466.70760239527</t>
+  </si>
+  <si>
+    <t>87469.48264991041</t>
   </si>
 </sst>
 </file>
@@ -910,7 +916,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:E22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1535,10 +1541,10 @@
         <v>172</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>177</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>178</v>
       </c>
       <c r="F22" t="s">
         <v>173</v>

</xml_diff>